<commit_message>
Minor changes and corrected text
</commit_message>
<xml_diff>
--- a/SponGIS_Template/SponGIS_Template.xlsx
+++ b/SponGIS_Template/SponGIS_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewdavies_mbp/Andy's Documents/Websites and comittees/SponGIS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewdavies_mbp/Andy's Documents/Websites and comittees/SponGIS/Github/SponGIS/SponGIS_Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="584">
   <si>
     <t>Class</t>
   </si>
@@ -1816,6 +1816,9 @@
   </si>
   <si>
     <t>Embargoed</t>
+  </si>
+  <si>
+    <t>The species schema standardises specific measurement data.</t>
   </si>
 </sst>
 </file>
@@ -2917,7 +2920,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3407,6 +3410,21 @@
     <xf numFmtId="14" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3419,21 +3437,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3456,9 +3459,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4929,7 +4929,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="96.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4946,10 +4946,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="237" t="s">
         <v>389</v>
       </c>
-      <c r="B1" s="239"/>
+      <c r="B1" s="237"/>
       <c r="D1" s="20" t="s">
         <v>163</v>
       </c>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="236" t="s">
-        <v>216</v>
+        <v>583</v>
       </c>
       <c r="B3" s="236"/>
       <c r="C3" s="236"/>
@@ -6143,8 +6143,8 @@
       <c r="A8" s="100" t="s">
         <v>452</v>
       </c>
-      <c r="B8" s="228"/>
-      <c r="C8" s="228"/>
+      <c r="B8" s="222"/>
+      <c r="C8" s="222"/>
       <c r="D8" s="118"/>
       <c r="E8" s="179" t="s">
         <v>580</v>
@@ -6163,8 +6163,8 @@
       <c r="A9" s="114" t="s">
         <v>454</v>
       </c>
-      <c r="B9" s="228"/>
-      <c r="C9" s="228"/>
+      <c r="B9" s="222"/>
+      <c r="C9" s="222"/>
       <c r="D9" s="118"/>
       <c r="E9" s="179" t="s">
         <v>579</v>
@@ -6179,11 +6179,11 @@
       <c r="A10" s="102" t="s">
         <v>461</v>
       </c>
-      <c r="B10" s="226"/>
-      <c r="C10" s="226"/>
-      <c r="D10" s="226"/>
-      <c r="E10" s="226"/>
-      <c r="F10" s="227"/>
+      <c r="B10" s="223"/>
+      <c r="C10" s="223"/>
+      <c r="D10" s="223"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="224"/>
       <c r="G10" s="101" t="s">
         <v>471</v>
       </c>
@@ -6193,11 +6193,11 @@
       <c r="A11" s="114" t="s">
         <v>460</v>
       </c>
-      <c r="B11" s="229"/>
-      <c r="C11" s="229"/>
-      <c r="D11" s="229"/>
-      <c r="E11" s="229"/>
-      <c r="F11" s="230"/>
+      <c r="B11" s="225"/>
+      <c r="C11" s="225"/>
+      <c r="D11" s="225"/>
+      <c r="E11" s="225"/>
+      <c r="F11" s="226"/>
       <c r="G11" s="101" t="s">
         <v>472</v>
       </c>
@@ -6207,11 +6207,11 @@
       <c r="A12" s="102" t="s">
         <v>458</v>
       </c>
-      <c r="B12" s="226"/>
-      <c r="C12" s="226"/>
-      <c r="D12" s="226"/>
-      <c r="E12" s="226"/>
-      <c r="F12" s="227"/>
+      <c r="B12" s="223"/>
+      <c r="C12" s="223"/>
+      <c r="D12" s="223"/>
+      <c r="E12" s="223"/>
+      <c r="F12" s="224"/>
       <c r="G12" s="101" t="s">
         <v>473</v>
       </c>
@@ -6221,11 +6221,11 @@
       <c r="A13" s="102" t="s">
         <v>457</v>
       </c>
-      <c r="B13" s="224"/>
-      <c r="C13" s="224"/>
-      <c r="D13" s="224"/>
-      <c r="E13" s="224"/>
-      <c r="F13" s="225"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="229"/>
+      <c r="D13" s="229"/>
+      <c r="E13" s="229"/>
+      <c r="F13" s="230"/>
       <c r="G13" s="101" t="s">
         <v>474</v>
       </c>
@@ -6233,11 +6233,11 @@
     </row>
     <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="102"/>
-      <c r="B14" s="224"/>
-      <c r="C14" s="224"/>
-      <c r="D14" s="224"/>
-      <c r="E14" s="224"/>
-      <c r="F14" s="225"/>
+      <c r="B14" s="229"/>
+      <c r="C14" s="229"/>
+      <c r="D14" s="229"/>
+      <c r="E14" s="229"/>
+      <c r="F14" s="230"/>
       <c r="G14" s="113" t="s">
         <v>475</v>
       </c>
@@ -6247,31 +6247,31 @@
       <c r="A15" s="117" t="s">
         <v>456</v>
       </c>
-      <c r="B15" s="224"/>
-      <c r="C15" s="224"/>
-      <c r="D15" s="224"/>
-      <c r="E15" s="224"/>
-      <c r="F15" s="225"/>
+      <c r="B15" s="229"/>
+      <c r="C15" s="229"/>
+      <c r="D15" s="229"/>
+      <c r="E15" s="229"/>
+      <c r="F15" s="230"/>
       <c r="G15" s="121"/>
       <c r="H15" s="119"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="117"/>
-      <c r="B16" s="224"/>
-      <c r="C16" s="224"/>
-      <c r="D16" s="224"/>
-      <c r="E16" s="224"/>
-      <c r="F16" s="225"/>
+      <c r="B16" s="229"/>
+      <c r="C16" s="229"/>
+      <c r="D16" s="229"/>
+      <c r="E16" s="229"/>
+      <c r="F16" s="230"/>
       <c r="G16" s="121"/>
       <c r="H16" s="119"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="117"/>
-      <c r="B17" s="224"/>
-      <c r="C17" s="224"/>
-      <c r="D17" s="224"/>
-      <c r="E17" s="224"/>
-      <c r="F17" s="225"/>
+      <c r="B17" s="229"/>
+      <c r="C17" s="229"/>
+      <c r="D17" s="229"/>
+      <c r="E17" s="229"/>
+      <c r="F17" s="230"/>
       <c r="G17" s="121"/>
       <c r="H17" s="119"/>
     </row>
@@ -6279,11 +6279,11 @@
       <c r="A18" s="103" t="s">
         <v>455</v>
       </c>
-      <c r="B18" s="222"/>
-      <c r="C18" s="222"/>
-      <c r="D18" s="222"/>
-      <c r="E18" s="222"/>
-      <c r="F18" s="223"/>
+      <c r="B18" s="227"/>
+      <c r="C18" s="227"/>
+      <c r="D18" s="227"/>
+      <c r="E18" s="227"/>
+      <c r="F18" s="228"/>
       <c r="G18" s="122"/>
       <c r="H18" s="120"/>
     </row>
@@ -6465,11 +6465,11 @@
       <c r="A8" s="102" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="224"/>
-      <c r="C8" s="224"/>
-      <c r="D8" s="224"/>
-      <c r="E8" s="224"/>
-      <c r="F8" s="224"/>
+      <c r="B8" s="229"/>
+      <c r="C8" s="229"/>
+      <c r="D8" s="229"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="229"/>
       <c r="G8" s="132"/>
       <c r="H8" s="44" t="s">
         <v>406</v>

</xml_diff>

<commit_message>
Added an "Advanced" version of sheet 3
The advanced version added to increase speed of data entry for users
that are confident with the Darwin Core terms used in the spreadsheet,
and as a result, will increase speed when entering large datasets.
</commit_message>
<xml_diff>
--- a/SponGIS_Template/SponGIS_Template.xlsx
+++ b/SponGIS_Template/SponGIS_Template.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="540" windowWidth="24520" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="6360" yWindow="2180" windowWidth="24520" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="13" r:id="rId1"/>
     <sheet name="1 Dataset Details" sheetId="14" r:id="rId2"/>
     <sheet name="2 Taxon Details" sheetId="18" r:id="rId3"/>
-    <sheet name="3 Event Details" sheetId="20" r:id="rId4"/>
-    <sheet name="Helpful-Additions" sheetId="21" r:id="rId5"/>
-    <sheet name="Help- Dataset" sheetId="8" r:id="rId6"/>
-    <sheet name="Help- Taxon" sheetId="10" r:id="rId7"/>
-    <sheet name="Help- Event" sheetId="9" r:id="rId8"/>
-    <sheet name="Help- ExtendedOccurrence" sheetId="11" r:id="rId9"/>
-    <sheet name="Help- ExtendedMeasurementOrFact" sheetId="12" r:id="rId10"/>
-    <sheet name="ContextDependents" sheetId="16" state="hidden" r:id="rId11"/>
+    <sheet name="3 Event Details Normal" sheetId="20" r:id="rId4"/>
+    <sheet name="3 Event Details Advanced" sheetId="22" r:id="rId5"/>
+    <sheet name="Helpful-Additions" sheetId="21" r:id="rId6"/>
+    <sheet name="Help- Dataset" sheetId="8" r:id="rId7"/>
+    <sheet name="Help- Taxon" sheetId="10" r:id="rId8"/>
+    <sheet name="Help- Event" sheetId="9" r:id="rId9"/>
+    <sheet name="Help- ExtendedOccurrence" sheetId="11" r:id="rId10"/>
+    <sheet name="Help- ExtendedMeasurementOrFact" sheetId="12" r:id="rId11"/>
+    <sheet name="ContextDependents" sheetId="16" state="hidden" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="CC">[1]Vocabularies!$G$2:$G$6</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="589">
   <si>
     <t>Class</t>
   </si>
@@ -1819,6 +1820,21 @@
   </si>
   <si>
     <t>The species schema standardises specific measurement data.</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>dataGeneralisations</t>
+  </si>
+  <si>
+    <t>fill in the advanced version of sheet</t>
+  </si>
+  <si>
+    <t>3, if not, then use the normal version.</t>
+  </si>
+  <si>
+    <t>If you feel confident with the terms,</t>
   </si>
 </sst>
 </file>
@@ -2157,7 +2173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="75">
     <border>
       <left/>
       <right/>
@@ -2809,6 +2825,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2920,7 +3114,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3290,6 +3484,36 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3322,33 +3546,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3437,18 +3634,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3461,6 +3658,78 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="69" xfId="107" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="72" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="73" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="74" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4069,7 +4338,7 @@
   <dimension ref="A1:AZ260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4098,16 +4367,16 @@
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
-      <c r="E2" s="195" t="s">
+      <c r="E2" s="185" t="s">
         <v>435</v>
       </c>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="185"/>
       <c r="M2" s="36"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -4115,14 +4384,14 @@
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="I3" s="195"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="195"/>
+      <c r="E3" s="185"/>
+      <c r="F3" s="185"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="185"/>
+      <c r="L3" s="185"/>
       <c r="M3" s="36"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -4162,16 +4431,16 @@
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="196" t="s">
+      <c r="E6" s="186" t="s">
         <v>437</v>
       </c>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="196"/>
-      <c r="I6" s="196"/>
-      <c r="J6" s="196"/>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
+      <c r="F6" s="186"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -4179,14 +4448,14 @@
       <c r="B7" s="36"/>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
-      <c r="E7" s="196"/>
-      <c r="F7" s="196"/>
-      <c r="G7" s="196"/>
-      <c r="H7" s="196"/>
-      <c r="I7" s="196"/>
-      <c r="J7" s="196"/>
-      <c r="K7" s="196"/>
-      <c r="L7" s="196"/>
+      <c r="E7" s="186"/>
+      <c r="F7" s="186"/>
+      <c r="G7" s="186"/>
+      <c r="H7" s="186"/>
+      <c r="I7" s="186"/>
+      <c r="J7" s="186"/>
+      <c r="K7" s="186"/>
+      <c r="L7" s="186"/>
       <c r="M7" s="36"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -4194,14 +4463,14 @@
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="196"/>
-      <c r="K8" s="196"/>
-      <c r="L8" s="196"/>
+      <c r="E8" s="186"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="186"/>
+      <c r="J8" s="186"/>
+      <c r="K8" s="186"/>
+      <c r="L8" s="186"/>
       <c r="M8" s="36"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -4357,19 +4626,19 @@
     <row r="18" spans="1:13" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
       <c r="B18" s="36"/>
-      <c r="C18" s="197" t="str">
+      <c r="C18" s="187" t="str">
         <f>IF(L17="Yes", "Enter the data ID to the box to the right, you can search for the value if you don't already have it at www.spongis.org/data-search/",IF(L17="No","Obtain a new data ID from, https://www.guidgenerator.com, no braces or hyphens please. Enter the value in the box to the right",""))</f>
         <v/>
       </c>
-      <c r="D18" s="198"/>
-      <c r="E18" s="198"/>
-      <c r="F18" s="198"/>
-      <c r="G18" s="198"/>
-      <c r="H18" s="198"/>
-      <c r="I18" s="198"/>
-      <c r="J18" s="199"/>
-      <c r="K18" s="200"/>
-      <c r="L18" s="201"/>
+      <c r="D18" s="188"/>
+      <c r="E18" s="188"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="188"/>
+      <c r="H18" s="188"/>
+      <c r="I18" s="188"/>
+      <c r="J18" s="189"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="191"/>
       <c r="M18" s="92"/>
     </row>
     <row r="19" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4407,17 +4676,17 @@
       <c r="B21" s="104" t="s">
         <v>440</v>
       </c>
-      <c r="C21" s="190" t="s">
+      <c r="C21" s="200" t="s">
         <v>449</v>
       </c>
-      <c r="D21" s="190"/>
-      <c r="E21" s="190"/>
-      <c r="F21" s="190"/>
-      <c r="G21" s="190"/>
-      <c r="H21" s="190"/>
-      <c r="I21" s="190"/>
-      <c r="J21" s="190"/>
-      <c r="K21" s="191"/>
+      <c r="D21" s="200"/>
+      <c r="E21" s="200"/>
+      <c r="F21" s="200"/>
+      <c r="G21" s="200"/>
+      <c r="H21" s="200"/>
+      <c r="I21" s="200"/>
+      <c r="J21" s="200"/>
+      <c r="K21" s="201"/>
       <c r="L21" s="105"/>
       <c r="M21" s="92">
         <f>IF(L21="Yes", 0.2,IF(L21="No",0.1,0))</f>
@@ -4469,8 +4738,8 @@
       <c r="H24" s="106"/>
       <c r="I24" s="106"/>
       <c r="J24" s="106"/>
-      <c r="K24" s="202"/>
-      <c r="L24" s="203"/>
+      <c r="K24" s="192"/>
+      <c r="L24" s="193"/>
       <c r="M24" s="92">
         <f>IF(K24="Species Occurrences", 10,IF(K24="Environmental data",20,IF(K24="Both",30,0)))</f>
         <v>0</v>
@@ -4520,12 +4789,12 @@
       <c r="G27" s="84"/>
       <c r="H27" s="84"/>
       <c r="I27" s="84"/>
-      <c r="J27" s="192" t="str">
+      <c r="J27" s="202" t="str">
         <f>IF(SUM(M17:M24)&gt;11,IF(M17=2,"1 - Dataset Details",IF(M17=1,"","")),"")</f>
         <v/>
       </c>
-      <c r="K27" s="193"/>
-      <c r="L27" s="194"/>
+      <c r="K27" s="203"/>
+      <c r="L27" s="204"/>
       <c r="M27" s="36"/>
     </row>
     <row r="28" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4538,12 +4807,12 @@
       <c r="G28" s="86"/>
       <c r="H28" s="86"/>
       <c r="I28" s="86"/>
-      <c r="J28" s="184" t="str">
+      <c r="J28" s="194" t="str">
         <f>IF(SUM(M17:M24)&gt;11,IF(M21=0.1,"2 - Taxon Details",IF(M21=0.2,"","")),"")</f>
         <v/>
       </c>
-      <c r="K28" s="185"/>
-      <c r="L28" s="186"/>
+      <c r="K28" s="195"/>
+      <c r="L28" s="196"/>
       <c r="M28" s="36"/>
     </row>
     <row r="29" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4553,15 +4822,17 @@
       <c r="D29" s="86"/>
       <c r="E29" s="86"/>
       <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="G29" s="275" t="s">
+        <v>588</v>
+      </c>
       <c r="H29" s="86"/>
       <c r="I29" s="86"/>
-      <c r="J29" s="184" t="str">
+      <c r="J29" s="194" t="str">
         <f>IF(SUM(M17:M24)&gt;11.1,"3 - Event Details","")</f>
         <v/>
       </c>
-      <c r="K29" s="185"/>
-      <c r="L29" s="186"/>
+      <c r="K29" s="195"/>
+      <c r="L29" s="196"/>
       <c r="M29" s="36"/>
     </row>
     <row r="30" spans="1:13" ht="21" x14ac:dyDescent="0.2">
@@ -4571,15 +4842,17 @@
       <c r="D30" s="86"/>
       <c r="E30" s="86"/>
       <c r="F30" s="86"/>
-      <c r="G30" s="86"/>
+      <c r="G30" s="275" t="s">
+        <v>586</v>
+      </c>
       <c r="H30" s="86"/>
       <c r="I30" s="86"/>
-      <c r="J30" s="184" t="str">
+      <c r="J30" s="194" t="str">
         <f>IF(SUM(M17:M24)&gt;10.1,IF(M24=10,"3a - Occurrence Details",IF(M24=30,"3a - Occurrence Details","")),"")</f>
         <v/>
       </c>
-      <c r="K30" s="185"/>
-      <c r="L30" s="186"/>
+      <c r="K30" s="195"/>
+      <c r="L30" s="196"/>
       <c r="M30" s="36"/>
     </row>
     <row r="31" spans="1:13" ht="22" thickBot="1" x14ac:dyDescent="0.25">
@@ -4589,15 +4862,17 @@
       <c r="D31" s="86"/>
       <c r="E31" s="86"/>
       <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
+      <c r="G31" s="275" t="s">
+        <v>587</v>
+      </c>
       <c r="H31" s="86"/>
       <c r="I31" s="86"/>
-      <c r="J31" s="187" t="str">
+      <c r="J31" s="197" t="str">
         <f>IF(SUM(M18:M26)&gt;10.1,IF(M24=20,"3b - Environmental Details",IF(M24=30,"3b - Environmmental Details","")),"")</f>
         <v/>
       </c>
-      <c r="K31" s="188"/>
-      <c r="L31" s="189"/>
+      <c r="K31" s="198"/>
+      <c r="L31" s="199"/>
       <c r="M31" s="36"/>
     </row>
     <row r="32" spans="1:13" ht="24" x14ac:dyDescent="0.3">
@@ -4879,17 +5154,17 @@
     <row r="260" s="36" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E2:L3"/>
-    <mergeCell ref="E6:L8"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="K24:L24"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="C21:K21"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="J28:L28"/>
     <mergeCell ref="J29:L29"/>
+    <mergeCell ref="E2:L3"/>
+    <mergeCell ref="E6:L8"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="K24:L24"/>
   </mergeCells>
   <conditionalFormatting sqref="J18:L18">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -4926,10 +5201,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="96.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4946,10 +5221,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
-        <v>389</v>
-      </c>
-      <c r="B1" s="237"/>
+      <c r="A1" s="238" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="238"/>
       <c r="D1" s="20" t="s">
         <v>163</v>
       </c>
@@ -4970,15 +5245,15 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="236" t="s">
-        <v>583</v>
-      </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
+      <c r="A3" s="237" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
@@ -5017,9 +5292,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>217</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>128</v>
@@ -5029,227 +5304,576 @@
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="21">
-        <v>1000</v>
-      </c>
+      <c r="H6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>296</v>
+      <c r="A8" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>401</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>162</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>296</v>
+        <v>112</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>391</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E9" s="18"/>
       <c r="F9" s="9" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>296</v>
+        <v>7</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>146</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>344</v>
+      </c>
       <c r="F10" s="9" t="s">
         <v>162</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" s="21" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>296</v>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="E11" s="18"/>
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="F11" s="9" t="s">
         <v>162</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="H11" s="21" t="s">
-        <v>395</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>296</v>
+      <c r="A12" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>396</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="H12" s="21" t="s">
-        <v>397</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>296</v>
+      <c r="A13" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>296</v>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>149</v>
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>348</v>
+      </c>
       <c r="F14" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="H14" s="21" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>296</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>152</v>
+        <v>58</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>404</v>
+        <v>350</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H15" s="21" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="H15" s="21">
+        <v>2008.1333999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="21" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>387</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5261,6 +5885,342 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="96.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12" style="9" customWidth="1"/>
+    <col min="7" max="7" width="66" style="1" customWidth="1"/>
+    <col min="8" max="8" width="76.33203125" style="21" customWidth="1"/>
+    <col min="9" max="16384" width="96.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="238" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" s="238"/>
+      <c r="D1" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="237" t="s">
+        <v>583</v>
+      </c>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="13" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
@@ -5426,11 +6386,11 @@
       <c r="G4" s="53"/>
       <c r="H4" s="54"/>
       <c r="I4" s="55"/>
-      <c r="J4" s="208" t="s">
+      <c r="J4" s="209" t="s">
         <v>427</v>
       </c>
-      <c r="K4" s="209"/>
-      <c r="L4" s="210"/>
+      <c r="K4" s="210"/>
+      <c r="L4" s="211"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="62"/>
@@ -5442,23 +6402,23 @@
       <c r="G5" s="40"/>
       <c r="H5" s="56"/>
       <c r="I5" s="50"/>
-      <c r="J5" s="211"/>
-      <c r="K5" s="212"/>
-      <c r="L5" s="213"/>
+      <c r="J5" s="212"/>
+      <c r="K5" s="213"/>
+      <c r="L5" s="214"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">
         <v>425</v>
       </c>
-      <c r="B6" s="218">
+      <c r="B6" s="219">
         <f>Instructions!J18</f>
         <v>0</v>
       </c>
-      <c r="C6" s="218"/>
-      <c r="D6" s="218"/>
-      <c r="E6" s="218"/>
-      <c r="F6" s="218"/>
-      <c r="G6" s="219"/>
+      <c r="C6" s="219"/>
+      <c r="D6" s="219"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="219"/>
+      <c r="G6" s="220"/>
       <c r="H6" s="56"/>
       <c r="I6" s="50"/>
       <c r="J6" s="58" t="s">
@@ -5475,12 +6435,12 @@
       <c r="A7" s="64" t="s">
         <v>431</v>
       </c>
-      <c r="B7" s="214"/>
-      <c r="C7" s="214"/>
-      <c r="D7" s="214"/>
-      <c r="E7" s="214"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="215"/>
+      <c r="B7" s="215"/>
+      <c r="C7" s="215"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="215"/>
+      <c r="F7" s="215"/>
+      <c r="G7" s="216"/>
       <c r="H7" s="56"/>
       <c r="I7" s="50"/>
       <c r="J7" s="59" t="s">
@@ -5493,12 +6453,12 @@
       <c r="A8" s="64" t="s">
         <v>432</v>
       </c>
-      <c r="B8" s="220"/>
-      <c r="C8" s="220"/>
-      <c r="D8" s="220"/>
-      <c r="E8" s="220"/>
-      <c r="F8" s="220"/>
-      <c r="G8" s="221"/>
+      <c r="B8" s="221"/>
+      <c r="C8" s="221"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="221"/>
+      <c r="F8" s="221"/>
+      <c r="G8" s="222"/>
       <c r="H8" s="56"/>
       <c r="I8" s="50"/>
       <c r="J8" s="60" t="s">
@@ -5511,12 +6471,12 @@
       <c r="A9" s="64" t="s">
         <v>433</v>
       </c>
-      <c r="B9" s="214"/>
-      <c r="C9" s="214"/>
-      <c r="D9" s="214"/>
-      <c r="E9" s="214"/>
-      <c r="F9" s="214"/>
-      <c r="G9" s="215"/>
+      <c r="B9" s="215"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
       <c r="J9" s="56"/>
@@ -5528,34 +6488,34 @@
       <c r="A10" s="68" t="s">
         <v>434</v>
       </c>
-      <c r="B10" s="216"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="217"/>
+      <c r="B10" s="217"/>
+      <c r="C10" s="217"/>
+      <c r="D10" s="217"/>
+      <c r="E10" s="217"/>
+      <c r="F10" s="217"/>
+      <c r="G10" s="218"/>
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
       <c r="J10" s="127" t="s">
         <v>480</v>
       </c>
-      <c r="K10" s="204" t="str">
+      <c r="K10" s="205" t="str">
         <f>CONCATENATE("POLYGON ((",L8,", ",L7,", ",K7,", ",K8,"))")</f>
         <v>POLYGON ((, , , ))</v>
       </c>
-      <c r="L10" s="205"/>
+      <c r="L10" s="206"/>
       <c r="M10" s="38"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="174" t="s">
         <v>581</v>
       </c>
-      <c r="B11" s="206"/>
-      <c r="C11" s="206"/>
-      <c r="D11" s="206"/>
-      <c r="E11" s="206"/>
-      <c r="F11" s="206"/>
-      <c r="G11" s="207"/>
+      <c r="B11" s="207"/>
+      <c r="C11" s="207"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="207"/>
+      <c r="G11" s="208"/>
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
       <c r="J11" s="56"/>
@@ -6143,8 +7103,8 @@
       <c r="A8" s="100" t="s">
         <v>452</v>
       </c>
-      <c r="B8" s="222"/>
-      <c r="C8" s="222"/>
+      <c r="B8" s="223"/>
+      <c r="C8" s="223"/>
       <c r="D8" s="118"/>
       <c r="E8" s="179" t="s">
         <v>580</v>
@@ -6163,8 +7123,8 @@
       <c r="A9" s="114" t="s">
         <v>454</v>
       </c>
-      <c r="B9" s="222"/>
-      <c r="C9" s="222"/>
+      <c r="B9" s="223"/>
+      <c r="C9" s="223"/>
       <c r="D9" s="118"/>
       <c r="E9" s="179" t="s">
         <v>579</v>
@@ -6179,11 +7139,11 @@
       <c r="A10" s="102" t="s">
         <v>461</v>
       </c>
-      <c r="B10" s="223"/>
-      <c r="C10" s="223"/>
-      <c r="D10" s="223"/>
-      <c r="E10" s="223"/>
-      <c r="F10" s="224"/>
+      <c r="B10" s="224"/>
+      <c r="C10" s="224"/>
+      <c r="D10" s="224"/>
+      <c r="E10" s="224"/>
+      <c r="F10" s="225"/>
       <c r="G10" s="101" t="s">
         <v>471</v>
       </c>
@@ -6193,11 +7153,11 @@
       <c r="A11" s="114" t="s">
         <v>460</v>
       </c>
-      <c r="B11" s="225"/>
-      <c r="C11" s="225"/>
-      <c r="D11" s="225"/>
-      <c r="E11" s="225"/>
-      <c r="F11" s="226"/>
+      <c r="B11" s="226"/>
+      <c r="C11" s="226"/>
+      <c r="D11" s="226"/>
+      <c r="E11" s="226"/>
+      <c r="F11" s="227"/>
       <c r="G11" s="101" t="s">
         <v>472</v>
       </c>
@@ -6207,11 +7167,11 @@
       <c r="A12" s="102" t="s">
         <v>458</v>
       </c>
-      <c r="B12" s="223"/>
-      <c r="C12" s="223"/>
-      <c r="D12" s="223"/>
-      <c r="E12" s="223"/>
-      <c r="F12" s="224"/>
+      <c r="B12" s="224"/>
+      <c r="C12" s="224"/>
+      <c r="D12" s="224"/>
+      <c r="E12" s="224"/>
+      <c r="F12" s="225"/>
       <c r="G12" s="101" t="s">
         <v>473</v>
       </c>
@@ -6221,11 +7181,11 @@
       <c r="A13" s="102" t="s">
         <v>457</v>
       </c>
-      <c r="B13" s="229"/>
-      <c r="C13" s="229"/>
-      <c r="D13" s="229"/>
-      <c r="E13" s="229"/>
-      <c r="F13" s="230"/>
+      <c r="B13" s="230"/>
+      <c r="C13" s="230"/>
+      <c r="D13" s="230"/>
+      <c r="E13" s="230"/>
+      <c r="F13" s="231"/>
       <c r="G13" s="101" t="s">
         <v>474</v>
       </c>
@@ -6233,11 +7193,11 @@
     </row>
     <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="102"/>
-      <c r="B14" s="229"/>
-      <c r="C14" s="229"/>
-      <c r="D14" s="229"/>
-      <c r="E14" s="229"/>
-      <c r="F14" s="230"/>
+      <c r="B14" s="230"/>
+      <c r="C14" s="230"/>
+      <c r="D14" s="230"/>
+      <c r="E14" s="230"/>
+      <c r="F14" s="231"/>
       <c r="G14" s="113" t="s">
         <v>475</v>
       </c>
@@ -6247,31 +7207,31 @@
       <c r="A15" s="117" t="s">
         <v>456</v>
       </c>
-      <c r="B15" s="229"/>
-      <c r="C15" s="229"/>
-      <c r="D15" s="229"/>
-      <c r="E15" s="229"/>
-      <c r="F15" s="230"/>
+      <c r="B15" s="230"/>
+      <c r="C15" s="230"/>
+      <c r="D15" s="230"/>
+      <c r="E15" s="230"/>
+      <c r="F15" s="231"/>
       <c r="G15" s="121"/>
       <c r="H15" s="119"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="117"/>
-      <c r="B16" s="229"/>
-      <c r="C16" s="229"/>
-      <c r="D16" s="229"/>
-      <c r="E16" s="229"/>
-      <c r="F16" s="230"/>
+      <c r="B16" s="230"/>
+      <c r="C16" s="230"/>
+      <c r="D16" s="230"/>
+      <c r="E16" s="230"/>
+      <c r="F16" s="231"/>
       <c r="G16" s="121"/>
       <c r="H16" s="119"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="117"/>
-      <c r="B17" s="229"/>
-      <c r="C17" s="229"/>
-      <c r="D17" s="229"/>
-      <c r="E17" s="229"/>
-      <c r="F17" s="230"/>
+      <c r="B17" s="230"/>
+      <c r="C17" s="230"/>
+      <c r="D17" s="230"/>
+      <c r="E17" s="230"/>
+      <c r="F17" s="231"/>
       <c r="G17" s="121"/>
       <c r="H17" s="119"/>
     </row>
@@ -6279,11 +7239,11 @@
       <c r="A18" s="103" t="s">
         <v>455</v>
       </c>
-      <c r="B18" s="227"/>
-      <c r="C18" s="227"/>
-      <c r="D18" s="227"/>
-      <c r="E18" s="227"/>
-      <c r="F18" s="228"/>
+      <c r="B18" s="228"/>
+      <c r="C18" s="228"/>
+      <c r="D18" s="228"/>
+      <c r="E18" s="228"/>
+      <c r="F18" s="229"/>
       <c r="G18" s="122"/>
       <c r="H18" s="120"/>
     </row>
@@ -6346,7 +7306,7 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6428,14 +7388,14 @@
       <c r="A6" s="115" t="s">
         <v>462</v>
       </c>
-      <c r="B6" s="231">
+      <c r="B6" s="234">
         <f>'1 Dataset Details'!$B$6:$G$6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="231"/>
-      <c r="D6" s="231"/>
-      <c r="E6" s="231"/>
-      <c r="F6" s="231"/>
+      <c r="C6" s="234"/>
+      <c r="D6" s="234"/>
+      <c r="E6" s="234"/>
+      <c r="F6" s="234"/>
       <c r="G6" s="147" t="s">
         <v>502</v>
       </c>
@@ -6449,11 +7409,11 @@
       <c r="A7" s="114" t="s">
         <v>429</v>
       </c>
-      <c r="B7" s="232"/>
-      <c r="C7" s="232"/>
-      <c r="D7" s="232"/>
-      <c r="E7" s="232"/>
-      <c r="F7" s="232"/>
+      <c r="B7" s="235"/>
+      <c r="C7" s="235"/>
+      <c r="D7" s="235"/>
+      <c r="E7" s="235"/>
+      <c r="F7" s="235"/>
       <c r="G7" s="132"/>
       <c r="H7" s="44" t="s">
         <v>505</v>
@@ -6465,11 +7425,11 @@
       <c r="A8" s="102" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="229"/>
-      <c r="C8" s="229"/>
-      <c r="D8" s="229"/>
-      <c r="E8" s="229"/>
-      <c r="F8" s="229"/>
+      <c r="B8" s="230"/>
+      <c r="C8" s="230"/>
+      <c r="D8" s="230"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="230"/>
       <c r="G8" s="132"/>
       <c r="H8" s="44" t="s">
         <v>406</v>
@@ -6481,9 +7441,9 @@
       <c r="A9" s="123" t="s">
         <v>476</v>
       </c>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
+      <c r="B9" s="232"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
       <c r="E9" s="131"/>
       <c r="F9" s="131"/>
       <c r="G9" s="149"/>
@@ -6497,11 +7457,11 @@
       <c r="A10" s="101" t="s">
         <v>497</v>
       </c>
-      <c r="B10" s="233"/>
-      <c r="C10" s="233"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="233"/>
-      <c r="F10" s="233"/>
+      <c r="B10" s="232"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="232"/>
       <c r="G10" s="145" t="s">
         <v>466</v>
       </c>
@@ -6515,11 +7475,11 @@
       <c r="A11" s="101" t="s">
         <v>499</v>
       </c>
-      <c r="B11" s="233"/>
-      <c r="C11" s="233"/>
-      <c r="D11" s="233"/>
-      <c r="E11" s="233"/>
-      <c r="F11" s="233"/>
+      <c r="B11" s="232"/>
+      <c r="C11" s="232"/>
+      <c r="D11" s="232"/>
+      <c r="E11" s="232"/>
+      <c r="F11" s="232"/>
       <c r="G11" s="132"/>
       <c r="H11" s="44" t="s">
         <v>507</v>
@@ -6531,11 +7491,11 @@
       <c r="A12" s="101" t="s">
         <v>500</v>
       </c>
-      <c r="B12" s="233"/>
-      <c r="C12" s="233"/>
-      <c r="D12" s="233"/>
-      <c r="E12" s="233"/>
-      <c r="F12" s="233"/>
+      <c r="B12" s="232"/>
+      <c r="C12" s="232"/>
+      <c r="D12" s="232"/>
+      <c r="E12" s="232"/>
+      <c r="F12" s="232"/>
       <c r="G12" s="176" t="s">
         <v>576</v>
       </c>
@@ -6549,11 +7509,11 @@
       <c r="A13" s="101" t="s">
         <v>498</v>
       </c>
-      <c r="B13" s="233"/>
-      <c r="C13" s="233"/>
-      <c r="D13" s="233"/>
-      <c r="E13" s="233"/>
-      <c r="F13" s="233"/>
+      <c r="B13" s="232"/>
+      <c r="C13" s="232"/>
+      <c r="D13" s="232"/>
+      <c r="E13" s="232"/>
+      <c r="F13" s="232"/>
       <c r="G13" s="132"/>
       <c r="H13" s="126" t="s">
         <v>41</v>
@@ -6565,11 +7525,11 @@
       <c r="A14" s="101" t="s">
         <v>501</v>
       </c>
-      <c r="B14" s="233"/>
-      <c r="C14" s="233"/>
-      <c r="D14" s="233"/>
-      <c r="E14" s="233"/>
-      <c r="F14" s="233"/>
+      <c r="B14" s="232"/>
+      <c r="C14" s="232"/>
+      <c r="D14" s="232"/>
+      <c r="E14" s="232"/>
+      <c r="F14" s="232"/>
       <c r="G14" s="132"/>
       <c r="H14" s="44" t="s">
         <v>509</v>
@@ -6579,11 +7539,11 @@
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="101"/>
-      <c r="B15" s="233"/>
-      <c r="C15" s="233"/>
-      <c r="D15" s="233"/>
-      <c r="E15" s="233"/>
-      <c r="F15" s="233"/>
+      <c r="B15" s="232"/>
+      <c r="C15" s="232"/>
+      <c r="D15" s="232"/>
+      <c r="E15" s="232"/>
+      <c r="F15" s="232"/>
       <c r="G15" s="149"/>
       <c r="H15" s="125" t="s">
         <v>510</v>
@@ -6595,11 +7555,11 @@
       <c r="A16" s="101" t="s">
         <v>520</v>
       </c>
-      <c r="B16" s="234"/>
-      <c r="C16" s="234"/>
-      <c r="D16" s="234"/>
-      <c r="E16" s="234"/>
-      <c r="F16" s="234"/>
+      <c r="B16" s="233"/>
+      <c r="C16" s="233"/>
+      <c r="D16" s="233"/>
+      <c r="E16" s="233"/>
+      <c r="F16" s="233"/>
       <c r="G16" s="132" t="s">
         <v>467</v>
       </c>
@@ -6611,11 +7571,11 @@
     </row>
     <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="160"/>
-      <c r="B17" s="234"/>
-      <c r="C17" s="234"/>
-      <c r="D17" s="234"/>
-      <c r="E17" s="234"/>
-      <c r="F17" s="234"/>
+      <c r="B17" s="233"/>
+      <c r="C17" s="233"/>
+      <c r="D17" s="233"/>
+      <c r="E17" s="233"/>
+      <c r="F17" s="233"/>
       <c r="G17" s="132"/>
       <c r="H17" s="44" t="s">
         <v>511</v>
@@ -6625,11 +7585,11 @@
     </row>
     <row r="18" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="112"/>
-      <c r="B18" s="234"/>
-      <c r="C18" s="234"/>
-      <c r="D18" s="234"/>
-      <c r="E18" s="234"/>
-      <c r="F18" s="234"/>
+      <c r="B18" s="233"/>
+      <c r="C18" s="233"/>
+      <c r="D18" s="233"/>
+      <c r="E18" s="233"/>
+      <c r="F18" s="233"/>
       <c r="G18" s="132"/>
       <c r="H18" s="44" t="s">
         <v>513</v>
@@ -7179,16 +8139,16 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="10">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B14:F15"/>
     <mergeCell ref="B16:F18"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <dataValidations count="56">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="eventID" prompt="An identifier for the set of information associated with an Event (something that occurs at a place and time)." sqref="B7:F7"/>
@@ -7276,6 +8236,535 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="1" tint="4.9989318521683403E-2"/>
+  </sheetPr>
+  <dimension ref="A1:BG7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="16.83203125" style="38" customWidth="1"/>
+    <col min="3" max="58" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="109" t="s">
+        <v>524</v>
+      </c>
+      <c r="E1" s="110" t="s">
+        <v>486</v>
+      </c>
+      <c r="J1" s="161" t="s">
+        <v>465</v>
+      </c>
+      <c r="K1" s="258"/>
+      <c r="L1" s="258"/>
+      <c r="M1" s="258"/>
+      <c r="N1" s="258"/>
+      <c r="O1" s="258"/>
+      <c r="P1" s="258"/>
+      <c r="Q1" s="258"/>
+      <c r="R1" s="258"/>
+      <c r="S1" s="258"/>
+      <c r="T1" s="258"/>
+      <c r="U1" s="258"/>
+      <c r="V1" s="258"/>
+      <c r="W1" s="258"/>
+      <c r="X1" s="262" t="s">
+        <v>521</v>
+      </c>
+      <c r="Y1" s="260"/>
+      <c r="Z1" s="260"/>
+      <c r="AA1" s="260"/>
+      <c r="AB1" s="260"/>
+      <c r="AC1" s="260"/>
+      <c r="AD1" s="260"/>
+      <c r="AE1" s="260"/>
+      <c r="AF1" s="260"/>
+      <c r="AG1" s="260"/>
+      <c r="AH1" s="260"/>
+      <c r="AI1" s="260"/>
+      <c r="AJ1" s="260"/>
+      <c r="AK1" s="260"/>
+      <c r="AL1" s="260"/>
+      <c r="AM1" s="260"/>
+      <c r="AN1" s="260"/>
+      <c r="AO1" s="260"/>
+      <c r="AP1" s="260"/>
+      <c r="AQ1" s="260"/>
+      <c r="AR1" s="260"/>
+      <c r="AS1" s="260"/>
+      <c r="AT1" s="260"/>
+      <c r="AU1" s="260"/>
+      <c r="AV1" s="260"/>
+      <c r="AW1" s="260"/>
+      <c r="AX1" s="262" t="s">
+        <v>558</v>
+      </c>
+      <c r="AY1" s="260"/>
+      <c r="AZ1" s="260"/>
+      <c r="BA1" s="260"/>
+      <c r="BB1" s="260"/>
+      <c r="BC1" s="260"/>
+      <c r="BD1" s="260"/>
+      <c r="BE1" s="260"/>
+      <c r="BF1" s="261"/>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A2" s="243" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="252"/>
+      <c r="J2" s="254" t="s">
+        <v>468</v>
+      </c>
+      <c r="K2" s="255"/>
+      <c r="L2" s="255"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="255"/>
+      <c r="O2" s="253" t="s">
+        <v>466</v>
+      </c>
+      <c r="P2" s="257" t="s">
+        <v>576</v>
+      </c>
+      <c r="Q2" s="255"/>
+      <c r="R2" s="255"/>
+      <c r="S2" s="255"/>
+      <c r="T2" s="256"/>
+      <c r="U2" s="259" t="s">
+        <v>467</v>
+      </c>
+      <c r="V2" s="260"/>
+      <c r="W2" s="260"/>
+      <c r="X2" s="263"/>
+      <c r="Y2" s="264"/>
+      <c r="Z2" s="264"/>
+      <c r="AA2" s="264"/>
+      <c r="AB2" s="264"/>
+      <c r="AC2" s="264"/>
+      <c r="AD2" s="264"/>
+      <c r="AE2" s="264"/>
+      <c r="AF2" s="264"/>
+      <c r="AG2" s="264"/>
+      <c r="AH2" s="264"/>
+      <c r="AI2" s="264"/>
+      <c r="AJ2" s="264"/>
+      <c r="AK2" s="264"/>
+      <c r="AL2" s="264"/>
+      <c r="AM2" s="264"/>
+      <c r="AN2" s="264"/>
+      <c r="AO2" s="264"/>
+      <c r="AP2" s="264"/>
+      <c r="AQ2" s="264"/>
+      <c r="AR2" s="264"/>
+      <c r="AS2" s="264"/>
+      <c r="AT2" s="264"/>
+      <c r="AU2" s="264"/>
+      <c r="AV2" s="264"/>
+      <c r="AW2" s="264"/>
+      <c r="AX2" s="263"/>
+      <c r="AY2" s="264"/>
+      <c r="AZ2" s="264"/>
+      <c r="BA2" s="264"/>
+      <c r="BB2" s="264"/>
+      <c r="BC2" s="264"/>
+      <c r="BD2" s="264"/>
+      <c r="BE2" s="264"/>
+      <c r="BF2" s="265"/>
+    </row>
+    <row r="3" spans="1:59" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="246" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="247" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="248" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="247" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="247" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="247" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="247" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="247" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="250" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="269" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="247" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="247" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="247" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="250" t="s">
+        <v>133</v>
+      </c>
+      <c r="O3" s="269" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="247" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="270" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="270" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="247" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" s="249" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="269" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="247" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="250" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="271" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="267" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="267" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA3" s="267" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB3" s="267" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="267" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD3" s="267" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE3" s="267" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF3" s="267" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG3" s="267" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH3" s="267" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI3" s="267" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ3" s="267" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK3" s="267" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL3" s="267" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM3" s="267" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN3" s="272" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" s="267" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP3" s="267" t="s">
+        <v>584</v>
+      </c>
+      <c r="AQ3" s="267" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR3" s="267" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS3" s="267" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT3" s="267" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU3" s="272" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV3" s="273" t="s">
+        <v>585</v>
+      </c>
+      <c r="AW3" s="274" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX3" s="266" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY3" s="267" t="s">
+        <v>142</v>
+      </c>
+      <c r="AZ3" s="267" t="s">
+        <v>136</v>
+      </c>
+      <c r="BA3" s="267" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB3" s="267" t="s">
+        <v>138</v>
+      </c>
+      <c r="BC3" s="267" t="s">
+        <v>139</v>
+      </c>
+      <c r="BD3" s="267" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE3" s="267" t="s">
+        <v>141</v>
+      </c>
+      <c r="BF3" s="268" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG3" s="50"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A4" s="240"/>
+      <c r="B4" s="184"/>
+      <c r="C4" s="241"/>
+      <c r="D4" s="241"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="241"/>
+      <c r="G4" s="241"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="242"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="251"/>
+      <c r="N4" s="251"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="251"/>
+      <c r="S4" s="251"/>
+      <c r="T4" s="251"/>
+      <c r="U4" s="251"/>
+      <c r="V4" s="251"/>
+      <c r="W4" s="251"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="47"/>
+      <c r="AL4" s="47"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="47"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="47"/>
+      <c r="AY4" s="47"/>
+      <c r="AZ4" s="47"/>
+      <c r="BA4" s="47"/>
+      <c r="BB4" s="47"/>
+      <c r="BC4" s="47"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="47"/>
+      <c r="BG4" s="50"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50"/>
+      <c r="AW5" s="50"/>
+      <c r="AX5" s="50"/>
+      <c r="AY5" s="50"/>
+      <c r="AZ5" s="50"/>
+      <c r="BA5" s="50"/>
+      <c r="BB5" s="50"/>
+      <c r="BC5" s="50"/>
+      <c r="BD5" s="50"/>
+      <c r="BE5" s="50"/>
+      <c r="BF5" s="50"/>
+      <c r="BG5" s="50"/>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="50"/>
+      <c r="X6" s="50"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="56">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementRemarks" prompt="Comments or notes accompanying the MeasurementOrFact, including if valid a link to the Pangaea archive for this dataset. Separate entries with ( | )." sqref="BF4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="dynamicProperties" prompt="A list (if more than one, separated with | ) of additional measurements, facts, characteristics, or assertions about the record. Meant to provide a mechanism for structured content such as key-value pairs (eg: &quot;{temperaturedegC:5} | {salinitypss:35}&quot;" sqref="AW4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="dataGeneralizations" prompt="Actions taken to make the shared data less specific or complete than in its original form. Suggests that alternative data of higher quality may be available on request." sqref="AV4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="collectionCode" prompt="The name, acronym, coden, or initialism identifying the collection or data set from which the record was derived." sqref="AT4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="modified" prompt="The most recent date-time on which the resource was changed." sqref="AS4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="associatedSequences" prompt="A list (concatenated and separated) of identifiers (publication, global unique identifier, URI) of genetic sequence information associated with the Occurrence." sqref="AR4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="associatedReferences" prompt="A list (concatenated and separated) of identifiers (publication, bibliographic reference, global unique identifier, URI) of literature associated with the Occurrence." sqref="AQ4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="associatedMedia" prompt="A list (concatenated and separated) of identifiers (publication, global unique identifier, URI) of media associated with the Occurrence." sqref="AP4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="preparations" prompt="A list (concatenated and separated) of preparations and preservation methods for a specimen." sqref="AO4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="establishmentMeans" prompt="The process by which the biological individual(s) represented in the Occurrence became established at the location." sqref="AM4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="lifeStage" prompt="The age class or life stage of the biological individual(s) at the time the Occurrence was recorded." sqref="AL4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="sex" prompt="The sex of the biological individual(s) represented in the Occurrence. " sqref="AK4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="organismQuantityType" prompt="The type of quantification system used for the quantity of organisms." sqref="AJ4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="organismQuantity" prompt="A number or enumeration value for the quantity of organisms." sqref="AI4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="recordedBy" prompt="A list (concatenated and separated) of names of people, groups, or organizations responsible for recording the original Occurrence. The primary collector or observer, especially one who applies a personal identifier (recordNumber), should be listed first" sqref="AH4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="occurrenceRemarks" prompt="Comments or notes about the Occurrence." sqref="AG4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="catalogNumber" prompt="An identifier (preferably unique) for the record within the data set or collection. Mostly for museum collections." sqref="AF4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="occurrenceID" prompt="An identifier for the Occurrence (as opposed to a particular digital record of the occurrence). In the absence of a persistent global unique identifier, construct one from a combination of identifiers in the record that will most closely make the occurren" sqref="Y4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="typeStatus" prompt="A list (if more than one, separated with | ) of nomenclatural types (type status, typified scientific name, publication) applied to the subject." sqref="AE4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="identificationQualifier" prompt="A brief phrase or a standard term (&quot;cf.&quot;, &quot;aff.&quot;) to express the determiner's doubts about the Identification." sqref="AD4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="identificationReferences" prompt="A list (if more than one separated with | ) of references (publication, global unique identifier, URI) used in the Identification." sqref="AB4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="identificationRemarks" prompt="Comments or notes about the Identification." sqref="AC4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="dateIdentified_x0009_" prompt="The date on which the subject was identified as representing the Taxon." sqref="AA4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="identifiedBy" prompt="A list (if more than one, separated with | ) of names of people, groups, or organizations who assigned the Taxon to the subject." sqref="Z4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="taxonID" prompt="An identifier for the set of taxon information (data associated with the Taxon class). May be a global unique identifier or an identifier specific to the data set. If possible match with OBIS." sqref="X4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementDeterminedBy" prompt="A list (if more than one, separated with | ) of names of people, groups, or organizations who determined the value of the MeasurementOrFact. " sqref="BE4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementDeterminedDate" prompt="The date on which the MeasurementOrFact was made. Recommended best practice is to use an encoding scheme, such as ISO 8601:2004(E)." sqref="BD4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementUnit" prompt="The units associated with the measurementValue. Recommended best practice is to use the International System of Units (SI). " sqref="BC4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementAccuracy" prompt="The description of the potential error associated with the measurementValue." sqref="BB4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementValue" prompt="The value of the measurement, fact, characteristic, or assertion." sqref="BA4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementType" prompt="The nature of the measurement, fact, characteristic, or assertion. e.g. &quot;Sea Surface Temperature&quot;." sqref="AZ4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementMethod" prompt="A description of or reference to (publication, URI) the method or protocol used to determine the measurement, fact, characteristic, or assertion._x000a_measurementType_x0009_The nature of the measurement, fact, characteristic, or assertion." sqref="AY4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="measurementID" prompt="An identifier for the MeasurementOrFact (information pertaining to measurements, facts, characteristics, or assertions). May be a global unique identifier or an identifier specific to the data set." sqref="AX4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="footprintWKT" prompt="Provide a shapefile name that will be converted into a Well-Known Text (WKT) representation of the shape (footprint, geometry) that defines the Location." sqref="W4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="locationRemarks" prompt="Comments or notes about the Location." sqref="V4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="locationAccordingTo" prompt="Information about the source of this Location information. Could be a publication (gazetteer), institution, or team of individuals. Likely Marine Regions." sqref="U4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="geodeticDatum" prompt="Spatial reference system (SRS) upon which the geographic coordinates given in decimalLatitude and decimalLongitude as based. Likely WGS 1984." sqref="T4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="coordinateUncertaintyInMeters" prompt="The horizontal distance (in meters) from the given decimalLatitude and decimalLongitude describing the smallest circle containing the whole of the Location." sqref="S4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="decimalLongitude" prompt="The geographic longitude (in decimal degrees, using the spatial reference system given in geodeticDatum) of the geographic center of a Location." sqref="R4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="decimalLatitude" prompt="The geographic latitude (in decimal degrees, using the spatial reference system given in geodeticDatum) of the geographic center of a Location." sqref="Q4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="maximumDepthInMeters" prompt="The greater depth of a range of depth below the local surface, in meters. If only 1 value provided, same for both min and max." sqref="P4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="minimumDepthInMeters" prompt="The lesser depth of a range of depth below the local surface, in meters. If only 1 value provided, same for both min and max." sqref="O4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="locality" prompt="The specific description or name of the place." sqref="N4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="country" prompt="The name of the country or major administrative unit in which the Location occurs." sqref="M4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="waterBody" prompt="The name of the water body in which the Location occurs." sqref="L4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="continent" prompt="The name of the continent in which the Location occurs." sqref="K4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="locationID" prompt="An identifier for the set of location information." sqref="J4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="habitat" prompt="A category or description of the habitat in which the Event occurred." sqref="I4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="eventRemarks" prompt="Comments or notes about the Event." sqref="H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="samplingEffort" prompt="The amount of effort expended during an Event." sqref="G4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="sampleSizeUnit" prompt="The unit of measurement of the size (time duration, length, area, or volume) of a sample in a sampling event." sqref="F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="sampleSizeValue" prompt="A numeric value for a measurement of the size (time duration, length, area, or volume) of a sample in a sampling event." sqref="E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="samplingProtocol" prompt="The name of, reference to, or description of the method or protocol used during an Event." sqref="D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="eventDate" prompt="The date-time or interval during which an Event occurred. For occurrences, this is the date-time when the event was recorded." sqref="C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="parentEventID" prompt="An identifier for the broader Event that groups this and potentially other Events. I.E. Could be a Cruise as a previous event, and then that becomes a Parent Event. Events do not need to have Occurrences or Measurements." sqref="B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="eventID" prompt="An identifier for the set of information associated with an Event (something that occurs at a place and time)." sqref="A4"/>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P2" location="'Helpful-Additions'!A1" display="Coord Converter"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="basisOfRecord" prompt="The specific nature of the data record. Select from Vocabulary">
+          <x14:formula1>
+            <xm:f>ContextDependents!$O$1:$O$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>AU4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="occurrenceStatus" prompt="A statement about the presence or absence of a Taxon at a Location.">
+          <x14:formula1>
+            <xm:f>ContextDependents!$M$1:$M$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>AN4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7415,7 +8904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -7437,10 +8926,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="236" t="s">
         <v>568</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="236"/>
       <c r="C1" s="28"/>
       <c r="D1" s="20" t="s">
         <v>163</v>
@@ -7459,15 +8948,15 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="237" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
@@ -7745,12 +9234,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="96.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7767,10 +9256,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="238" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="237"/>
+      <c r="B1" s="238"/>
       <c r="D1" s="20" t="s">
         <v>163</v>
       </c>
@@ -7791,15 +9280,15 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="237" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
@@ -8193,7 +9682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
@@ -8215,10 +9704,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="239" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="238"/>
+      <c r="B1" s="239"/>
       <c r="D1" s="20" t="s">
         <v>163</v>
       </c>
@@ -8239,15 +9728,15 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="237" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
@@ -8850,691 +10339,6 @@
       </c>
       <c r="H29" s="21" t="s">
         <v>331</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:G3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="96.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12" style="9" customWidth="1"/>
-    <col min="7" max="7" width="66" style="1" customWidth="1"/>
-    <col min="8" max="8" width="76.33203125" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="96.6640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
-        <v>388</v>
-      </c>
-      <c r="B1" s="237"/>
-      <c r="D1" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="236" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236"/>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" s="13" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="34"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
-    </row>
-    <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H15" s="21">
-        <v>2008.1333999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="112" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="144" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>